<commit_message>
Before convert to pack structure.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -17,13 +17,17 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="000000FF"/>
+      <u val="single"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +50,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,206 +447,53 @@
           <t>المدينة</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>الصورة الشخصية</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>الجنس</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>asd</t>
+          <t>عبد المجيد</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>asd</t>
+          <t>الشامي</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>asd</t>
+          <t>9999</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>اللاذقية</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>حلب</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>sdfa</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>اللاذقية</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>sadf</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>sdf</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>اللاذقية</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>ASDF</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>اللاذقية</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>اللاذقية</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> asdf</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>حلب</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>اللاذقية</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>شسي</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>شسي</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>شسي</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>طرطوس</t>
+          <t>حمص</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>عرض الصورة</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>ذكر</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>